<commit_message>
Raduls linear test with 12 threads
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\Studia\RADULS-master_my\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3281083-A44D-4663-9BA1-7B78B6BA4768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F267CF9-9ADC-4FA8-A98F-2B59534E7C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Thread_comp_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Thread_comp_2" sheetId="3" r:id="rId2"/>
-    <sheet name="Thread_comp_3" sheetId="4" r:id="rId3"/>
-    <sheet name="One_thread_linear" sheetId="2" r:id="rId4"/>
-    <sheet name="One_thread_log" sheetId="5" r:id="rId5"/>
+    <sheet name="Arkusz1" sheetId="6" r:id="rId1"/>
+    <sheet name="Thread_comp_1" sheetId="1" r:id="rId2"/>
+    <sheet name="Thread_comp_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Thread_comp_3" sheetId="4" r:id="rId4"/>
+    <sheet name="One_thread_linear" sheetId="2" r:id="rId5"/>
+    <sheet name="One_thread_log" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>seconds</t>
   </si>
@@ -87,6 +88,42 @@
   <si>
     <t>Raduls_sort;lengthmin=400;lengthmax=10485760000;lengtstep=0;lengtmult=2;num_threads=12;testite=1</t>
   </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=2;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=3;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=4;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=5;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=6;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=7;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=8;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=9;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=10;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=11;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;num_threads=12;testite=1</t>
+  </si>
+  <si>
+    <t>Raduls_sort;lengthmin=16384;lengthmax=536870912;lengtstep=0;lengtmult=2;testite=1</t>
+  </si>
 </sst>
 </file>
 
@@ -121,8 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -16754,6 +16792,1322 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2521F7E2-4849-40EA-A3C2-3E216DE6C759}">
+  <dimension ref="A1:X20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A1:X20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.0410000000000003E-3</v>
+      </c>
+      <c r="B3">
+        <v>16384</v>
+      </c>
+      <c r="C3">
+        <v>6.9049999999999997E-3</v>
+      </c>
+      <c r="D3">
+        <v>16384</v>
+      </c>
+      <c r="E3">
+        <v>8.6730000000000002E-3</v>
+      </c>
+      <c r="F3">
+        <v>16384</v>
+      </c>
+      <c r="G3">
+        <v>1.0952999999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>16384</v>
+      </c>
+      <c r="I3">
+        <v>1.3786E-2</v>
+      </c>
+      <c r="J3">
+        <v>16384</v>
+      </c>
+      <c r="K3">
+        <v>1.3774E-2</v>
+      </c>
+      <c r="L3">
+        <v>16384</v>
+      </c>
+      <c r="M3">
+        <v>1.4389000000000001E-2</v>
+      </c>
+      <c r="N3">
+        <v>16384</v>
+      </c>
+      <c r="O3">
+        <v>1.7336000000000001E-2</v>
+      </c>
+      <c r="P3">
+        <v>16384</v>
+      </c>
+      <c r="Q3">
+        <v>1.8683000000000002E-2</v>
+      </c>
+      <c r="R3">
+        <v>16384</v>
+      </c>
+      <c r="S3">
+        <v>1.9257E-2</v>
+      </c>
+      <c r="T3">
+        <v>16384</v>
+      </c>
+      <c r="U3">
+        <v>2.1356E-2</v>
+      </c>
+      <c r="V3">
+        <v>16384</v>
+      </c>
+      <c r="W3">
+        <v>2.5020000000000001E-2</v>
+      </c>
+      <c r="X3">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.8729999999999997E-3</v>
+      </c>
+      <c r="B4">
+        <v>32768</v>
+      </c>
+      <c r="C4">
+        <v>4.8729999999999997E-3</v>
+      </c>
+      <c r="D4">
+        <v>32768</v>
+      </c>
+      <c r="E4">
+        <v>6.4929999999999996E-3</v>
+      </c>
+      <c r="F4">
+        <v>32768</v>
+      </c>
+      <c r="G4">
+        <v>8.4849999999999995E-3</v>
+      </c>
+      <c r="H4">
+        <v>32768</v>
+      </c>
+      <c r="I4">
+        <v>1.157E-2</v>
+      </c>
+      <c r="J4">
+        <v>32768</v>
+      </c>
+      <c r="K4">
+        <v>1.2319999999999999E-2</v>
+      </c>
+      <c r="L4">
+        <v>32768</v>
+      </c>
+      <c r="M4">
+        <v>1.5043000000000001E-2</v>
+      </c>
+      <c r="N4">
+        <v>32768</v>
+      </c>
+      <c r="O4">
+        <v>1.6233000000000001E-2</v>
+      </c>
+      <c r="P4">
+        <v>32768</v>
+      </c>
+      <c r="Q4">
+        <v>1.8162999999999999E-2</v>
+      </c>
+      <c r="R4">
+        <v>32768</v>
+      </c>
+      <c r="S4">
+        <v>1.9737999999999999E-2</v>
+      </c>
+      <c r="T4">
+        <v>32768</v>
+      </c>
+      <c r="U4">
+        <v>2.2350999999999999E-2</v>
+      </c>
+      <c r="V4">
+        <v>32768</v>
+      </c>
+      <c r="W4">
+        <v>2.5069000000000001E-2</v>
+      </c>
+      <c r="X4">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.2820000000000003E-3</v>
+      </c>
+      <c r="B5">
+        <v>65536</v>
+      </c>
+      <c r="C5">
+        <v>6.012E-3</v>
+      </c>
+      <c r="D5">
+        <v>65536</v>
+      </c>
+      <c r="E5">
+        <v>7.6249999999999998E-3</v>
+      </c>
+      <c r="F5">
+        <v>65536</v>
+      </c>
+      <c r="G5">
+        <v>1.0949E-2</v>
+      </c>
+      <c r="H5">
+        <v>65536</v>
+      </c>
+      <c r="I5">
+        <v>1.0521000000000001E-2</v>
+      </c>
+      <c r="J5">
+        <v>65536</v>
+      </c>
+      <c r="K5">
+        <v>1.1708E-2</v>
+      </c>
+      <c r="L5">
+        <v>65536</v>
+      </c>
+      <c r="M5">
+        <v>1.4322E-2</v>
+      </c>
+      <c r="N5">
+        <v>65536</v>
+      </c>
+      <c r="O5">
+        <v>1.7052000000000001E-2</v>
+      </c>
+      <c r="P5">
+        <v>65536</v>
+      </c>
+      <c r="Q5">
+        <v>1.7662000000000001E-2</v>
+      </c>
+      <c r="R5">
+        <v>65536</v>
+      </c>
+      <c r="S5">
+        <v>1.8974999999999999E-2</v>
+      </c>
+      <c r="T5">
+        <v>65536</v>
+      </c>
+      <c r="U5">
+        <v>2.0312E-2</v>
+      </c>
+      <c r="V5">
+        <v>65536</v>
+      </c>
+      <c r="W5">
+        <v>2.2297999999999998E-2</v>
+      </c>
+      <c r="X5">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.0782999999999999E-2</v>
+      </c>
+      <c r="B6">
+        <v>131072</v>
+      </c>
+      <c r="C6">
+        <v>1.0591E-2</v>
+      </c>
+      <c r="D6">
+        <v>131072</v>
+      </c>
+      <c r="E6">
+        <v>9.3270000000000002E-3</v>
+      </c>
+      <c r="F6">
+        <v>131072</v>
+      </c>
+      <c r="G6">
+        <v>1.0829E-2</v>
+      </c>
+      <c r="H6">
+        <v>131072</v>
+      </c>
+      <c r="I6">
+        <v>1.0604000000000001E-2</v>
+      </c>
+      <c r="J6">
+        <v>131072</v>
+      </c>
+      <c r="K6">
+        <v>1.2605E-2</v>
+      </c>
+      <c r="L6">
+        <v>131072</v>
+      </c>
+      <c r="M6">
+        <v>1.4408000000000001E-2</v>
+      </c>
+      <c r="N6">
+        <v>131072</v>
+      </c>
+      <c r="O6">
+        <v>1.5317000000000001E-2</v>
+      </c>
+      <c r="P6">
+        <v>131072</v>
+      </c>
+      <c r="Q6">
+        <v>1.6739E-2</v>
+      </c>
+      <c r="R6">
+        <v>131072</v>
+      </c>
+      <c r="S6">
+        <v>1.8970999999999998E-2</v>
+      </c>
+      <c r="T6">
+        <v>131072</v>
+      </c>
+      <c r="U6">
+        <v>2.0258999999999999E-2</v>
+      </c>
+      <c r="V6">
+        <v>131072</v>
+      </c>
+      <c r="W6">
+        <v>2.2085E-2</v>
+      </c>
+      <c r="X6">
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.9063E-2</v>
+      </c>
+      <c r="B7">
+        <v>262144</v>
+      </c>
+      <c r="C7">
+        <v>1.1915E-2</v>
+      </c>
+      <c r="D7">
+        <v>262144</v>
+      </c>
+      <c r="E7">
+        <v>1.0663000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>262144</v>
+      </c>
+      <c r="G7">
+        <v>1.1448E-2</v>
+      </c>
+      <c r="H7">
+        <v>262144</v>
+      </c>
+      <c r="I7">
+        <v>1.2107E-2</v>
+      </c>
+      <c r="J7">
+        <v>262144</v>
+      </c>
+      <c r="K7">
+        <v>1.3599E-2</v>
+      </c>
+      <c r="L7">
+        <v>262144</v>
+      </c>
+      <c r="M7">
+        <v>1.4985999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>262144</v>
+      </c>
+      <c r="O7">
+        <v>1.9028E-2</v>
+      </c>
+      <c r="P7">
+        <v>262144</v>
+      </c>
+      <c r="Q7">
+        <v>1.8435E-2</v>
+      </c>
+      <c r="R7">
+        <v>262144</v>
+      </c>
+      <c r="S7">
+        <v>2.2638999999999999E-2</v>
+      </c>
+      <c r="T7">
+        <v>262144</v>
+      </c>
+      <c r="U7">
+        <v>2.4341999999999999E-2</v>
+      </c>
+      <c r="V7">
+        <v>262144</v>
+      </c>
+      <c r="W7">
+        <v>2.3005999999999999E-2</v>
+      </c>
+      <c r="X7">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.3144000000000002E-2</v>
+      </c>
+      <c r="B8">
+        <v>524288</v>
+      </c>
+      <c r="C8">
+        <v>2.2974999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>524288</v>
+      </c>
+      <c r="E8">
+        <v>1.7947999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <v>524288</v>
+      </c>
+      <c r="G8">
+        <v>1.6404999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>524288</v>
+      </c>
+      <c r="I8">
+        <v>1.8090999999999999E-2</v>
+      </c>
+      <c r="J8">
+        <v>524288</v>
+      </c>
+      <c r="K8">
+        <v>1.8475999999999999E-2</v>
+      </c>
+      <c r="L8">
+        <v>524288</v>
+      </c>
+      <c r="M8">
+        <v>1.9255000000000001E-2</v>
+      </c>
+      <c r="N8">
+        <v>524288</v>
+      </c>
+      <c r="O8">
+        <v>2.044E-2</v>
+      </c>
+      <c r="P8">
+        <v>524288</v>
+      </c>
+      <c r="Q8">
+        <v>2.3373000000000001E-2</v>
+      </c>
+      <c r="R8">
+        <v>524288</v>
+      </c>
+      <c r="S8">
+        <v>2.3540999999999999E-2</v>
+      </c>
+      <c r="T8">
+        <v>524288</v>
+      </c>
+      <c r="U8">
+        <v>2.5870000000000001E-2</v>
+      </c>
+      <c r="V8">
+        <v>524288</v>
+      </c>
+      <c r="W8">
+        <v>2.7226E-2</v>
+      </c>
+      <c r="X8">
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.10369100000000001</v>
+      </c>
+      <c r="B9">
+        <v>1048576</v>
+      </c>
+      <c r="C9">
+        <v>5.4975000000000003E-2</v>
+      </c>
+      <c r="D9">
+        <v>1048576</v>
+      </c>
+      <c r="E9">
+        <v>3.7193999999999998E-2</v>
+      </c>
+      <c r="F9">
+        <v>1048576</v>
+      </c>
+      <c r="G9">
+        <v>3.6748000000000003E-2</v>
+      </c>
+      <c r="H9">
+        <v>1048576</v>
+      </c>
+      <c r="I9">
+        <v>3.2327000000000002E-2</v>
+      </c>
+      <c r="J9">
+        <v>1048576</v>
+      </c>
+      <c r="K9">
+        <v>2.9481E-2</v>
+      </c>
+      <c r="L9">
+        <v>1048576</v>
+      </c>
+      <c r="M9">
+        <v>3.3536999999999997E-2</v>
+      </c>
+      <c r="N9">
+        <v>1048576</v>
+      </c>
+      <c r="O9">
+        <v>3.0689999999999999E-2</v>
+      </c>
+      <c r="P9">
+        <v>1048576</v>
+      </c>
+      <c r="Q9">
+        <v>3.1185999999999998E-2</v>
+      </c>
+      <c r="R9">
+        <v>1048576</v>
+      </c>
+      <c r="S9">
+        <v>3.2036000000000002E-2</v>
+      </c>
+      <c r="T9">
+        <v>1048576</v>
+      </c>
+      <c r="U9">
+        <v>3.6326999999999998E-2</v>
+      </c>
+      <c r="V9">
+        <v>1048576</v>
+      </c>
+      <c r="W9">
+        <v>3.4390999999999998E-2</v>
+      </c>
+      <c r="X9">
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.35982700000000001</v>
+      </c>
+      <c r="B10">
+        <v>2097152</v>
+      </c>
+      <c r="C10">
+        <v>0.14945600000000001</v>
+      </c>
+      <c r="D10">
+        <v>2097152</v>
+      </c>
+      <c r="E10">
+        <v>0.104338</v>
+      </c>
+      <c r="F10">
+        <v>2097152</v>
+      </c>
+      <c r="G10">
+        <v>9.5120999999999997E-2</v>
+      </c>
+      <c r="H10">
+        <v>2097152</v>
+      </c>
+      <c r="I10">
+        <v>7.9718999999999998E-2</v>
+      </c>
+      <c r="J10">
+        <v>2097152</v>
+      </c>
+      <c r="K10">
+        <v>6.7847000000000005E-2</v>
+      </c>
+      <c r="L10">
+        <v>2097152</v>
+      </c>
+      <c r="M10">
+        <v>6.7139000000000004E-2</v>
+      </c>
+      <c r="N10">
+        <v>2097152</v>
+      </c>
+      <c r="O10">
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="P10">
+        <v>2097152</v>
+      </c>
+      <c r="Q10">
+        <v>6.2265000000000001E-2</v>
+      </c>
+      <c r="R10">
+        <v>2097152</v>
+      </c>
+      <c r="S10">
+        <v>6.2079000000000002E-2</v>
+      </c>
+      <c r="T10">
+        <v>2097152</v>
+      </c>
+      <c r="U10">
+        <v>6.2497999999999998E-2</v>
+      </c>
+      <c r="V10">
+        <v>2097152</v>
+      </c>
+      <c r="W10">
+        <v>6.1565000000000002E-2</v>
+      </c>
+      <c r="X10">
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.244924</v>
+      </c>
+      <c r="B11">
+        <v>4194304</v>
+      </c>
+      <c r="C11">
+        <v>0.12564500000000001</v>
+      </c>
+      <c r="D11">
+        <v>4194304</v>
+      </c>
+      <c r="E11">
+        <v>8.7347999999999995E-2</v>
+      </c>
+      <c r="F11">
+        <v>4194304</v>
+      </c>
+      <c r="G11">
+        <v>7.4028999999999998E-2</v>
+      </c>
+      <c r="H11">
+        <v>4194304</v>
+      </c>
+      <c r="I11">
+        <v>6.0456999999999997E-2</v>
+      </c>
+      <c r="J11">
+        <v>4194304</v>
+      </c>
+      <c r="K11">
+        <v>6.1532999999999997E-2</v>
+      </c>
+      <c r="L11">
+        <v>4194304</v>
+      </c>
+      <c r="M11">
+        <v>5.7835999999999999E-2</v>
+      </c>
+      <c r="N11">
+        <v>4194304</v>
+      </c>
+      <c r="O11">
+        <v>5.6750000000000002E-2</v>
+      </c>
+      <c r="P11">
+        <v>4194304</v>
+      </c>
+      <c r="Q11">
+        <v>5.4923E-2</v>
+      </c>
+      <c r="R11">
+        <v>4194304</v>
+      </c>
+      <c r="S11">
+        <v>5.6668000000000003E-2</v>
+      </c>
+      <c r="T11">
+        <v>4194304</v>
+      </c>
+      <c r="U11">
+        <v>5.6610000000000001E-2</v>
+      </c>
+      <c r="V11">
+        <v>4194304</v>
+      </c>
+      <c r="W11">
+        <v>5.9381999999999997E-2</v>
+      </c>
+      <c r="X11">
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.43234299999999998</v>
+      </c>
+      <c r="B12">
+        <v>8388608</v>
+      </c>
+      <c r="C12">
+        <v>0.224082</v>
+      </c>
+      <c r="D12">
+        <v>8388608</v>
+      </c>
+      <c r="E12">
+        <v>0.15298600000000001</v>
+      </c>
+      <c r="F12">
+        <v>8388608</v>
+      </c>
+      <c r="G12">
+        <v>0.12531</v>
+      </c>
+      <c r="H12">
+        <v>8388608</v>
+      </c>
+      <c r="I12">
+        <v>0.107806</v>
+      </c>
+      <c r="J12">
+        <v>8388608</v>
+      </c>
+      <c r="K12">
+        <v>0.107062</v>
+      </c>
+      <c r="L12">
+        <v>8388608</v>
+      </c>
+      <c r="M12">
+        <v>9.0507000000000004E-2</v>
+      </c>
+      <c r="N12">
+        <v>8388608</v>
+      </c>
+      <c r="O12">
+        <v>8.4758E-2</v>
+      </c>
+      <c r="P12">
+        <v>8388608</v>
+      </c>
+      <c r="Q12">
+        <v>9.2567999999999998E-2</v>
+      </c>
+      <c r="R12">
+        <v>8388608</v>
+      </c>
+      <c r="S12">
+        <v>8.4316000000000002E-2</v>
+      </c>
+      <c r="T12">
+        <v>8388608</v>
+      </c>
+      <c r="U12">
+        <v>8.2794000000000006E-2</v>
+      </c>
+      <c r="V12">
+        <v>8388608</v>
+      </c>
+      <c r="W12">
+        <v>8.8747000000000006E-2</v>
+      </c>
+      <c r="X12">
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.941415</v>
+      </c>
+      <c r="B13">
+        <v>16777216</v>
+      </c>
+      <c r="C13">
+        <v>0.50962200000000002</v>
+      </c>
+      <c r="D13">
+        <v>16777216</v>
+      </c>
+      <c r="E13">
+        <v>0.34367700000000001</v>
+      </c>
+      <c r="F13">
+        <v>16777216</v>
+      </c>
+      <c r="G13">
+        <v>0.26515699999999998</v>
+      </c>
+      <c r="H13">
+        <v>16777216</v>
+      </c>
+      <c r="I13">
+        <v>0.22494900000000001</v>
+      </c>
+      <c r="J13">
+        <v>16777216</v>
+      </c>
+      <c r="K13">
+        <v>0.200155</v>
+      </c>
+      <c r="L13">
+        <v>16777216</v>
+      </c>
+      <c r="M13">
+        <v>0.183502</v>
+      </c>
+      <c r="N13">
+        <v>16777216</v>
+      </c>
+      <c r="O13">
+        <v>0.19080800000000001</v>
+      </c>
+      <c r="P13">
+        <v>16777216</v>
+      </c>
+      <c r="Q13">
+        <v>0.167964</v>
+      </c>
+      <c r="R13">
+        <v>16777216</v>
+      </c>
+      <c r="S13">
+        <v>0.16383500000000001</v>
+      </c>
+      <c r="T13">
+        <v>16777216</v>
+      </c>
+      <c r="U13">
+        <v>0.16646900000000001</v>
+      </c>
+      <c r="V13">
+        <v>16777216</v>
+      </c>
+      <c r="W13">
+        <v>0.153063</v>
+      </c>
+      <c r="X13">
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2.1475569999999999</v>
+      </c>
+      <c r="B14">
+        <v>33554432</v>
+      </c>
+      <c r="C14">
+        <v>1.096681</v>
+      </c>
+      <c r="D14">
+        <v>33554432</v>
+      </c>
+      <c r="E14">
+        <v>0.78250299999999995</v>
+      </c>
+      <c r="F14">
+        <v>33554432</v>
+      </c>
+      <c r="G14">
+        <v>0.59825600000000001</v>
+      </c>
+      <c r="H14">
+        <v>33554432</v>
+      </c>
+      <c r="I14">
+        <v>0.48775600000000002</v>
+      </c>
+      <c r="J14">
+        <v>33554432</v>
+      </c>
+      <c r="K14">
+        <v>0.43679200000000001</v>
+      </c>
+      <c r="L14">
+        <v>33554432</v>
+      </c>
+      <c r="M14">
+        <v>0.41364000000000001</v>
+      </c>
+      <c r="N14">
+        <v>33554432</v>
+      </c>
+      <c r="O14">
+        <v>0.382766</v>
+      </c>
+      <c r="P14">
+        <v>33554432</v>
+      </c>
+      <c r="Q14">
+        <v>0.36288100000000001</v>
+      </c>
+      <c r="R14">
+        <v>33554432</v>
+      </c>
+      <c r="S14">
+        <v>0.35128700000000002</v>
+      </c>
+      <c r="T14">
+        <v>33554432</v>
+      </c>
+      <c r="U14">
+        <v>0.33320699999999998</v>
+      </c>
+      <c r="V14">
+        <v>33554432</v>
+      </c>
+      <c r="W14">
+        <v>0.32631399999999999</v>
+      </c>
+      <c r="X14">
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.8858819999999996</v>
+      </c>
+      <c r="B15">
+        <v>67108864</v>
+      </c>
+      <c r="C15">
+        <v>2.530621</v>
+      </c>
+      <c r="D15">
+        <v>67108864</v>
+      </c>
+      <c r="E15">
+        <v>1.777523</v>
+      </c>
+      <c r="F15">
+        <v>67108864</v>
+      </c>
+      <c r="G15">
+        <v>1.37052</v>
+      </c>
+      <c r="H15">
+        <v>67108864</v>
+      </c>
+      <c r="I15">
+        <v>1.155761</v>
+      </c>
+      <c r="J15">
+        <v>67108864</v>
+      </c>
+      <c r="K15">
+        <v>0.99126300000000001</v>
+      </c>
+      <c r="L15">
+        <v>67108864</v>
+      </c>
+      <c r="M15">
+        <v>0.95729799999999998</v>
+      </c>
+      <c r="N15">
+        <v>67108864</v>
+      </c>
+      <c r="O15">
+        <v>0.84314</v>
+      </c>
+      <c r="P15">
+        <v>67108864</v>
+      </c>
+      <c r="Q15">
+        <v>0.82293700000000003</v>
+      </c>
+      <c r="R15">
+        <v>67108864</v>
+      </c>
+      <c r="S15">
+        <v>0.76904899999999998</v>
+      </c>
+      <c r="T15">
+        <v>67108864</v>
+      </c>
+      <c r="U15">
+        <v>0.76454800000000001</v>
+      </c>
+      <c r="V15">
+        <v>67108864</v>
+      </c>
+      <c r="W15">
+        <v>0.756745</v>
+      </c>
+      <c r="X15">
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11.292381000000001</v>
+      </c>
+      <c r="B16">
+        <v>134217728</v>
+      </c>
+      <c r="C16">
+        <v>5.8051680000000001</v>
+      </c>
+      <c r="D16">
+        <v>134217728</v>
+      </c>
+      <c r="E16">
+        <v>4.1215000000000002</v>
+      </c>
+      <c r="F16">
+        <v>134217728</v>
+      </c>
+      <c r="G16">
+        <v>3.1470739999999999</v>
+      </c>
+      <c r="H16">
+        <v>134217728</v>
+      </c>
+      <c r="I16">
+        <v>2.6295039999999998</v>
+      </c>
+      <c r="J16">
+        <v>134217728</v>
+      </c>
+      <c r="K16">
+        <v>2.3019759999999998</v>
+      </c>
+      <c r="L16">
+        <v>134217728</v>
+      </c>
+      <c r="M16">
+        <v>2.1281319999999999</v>
+      </c>
+      <c r="N16">
+        <v>134217728</v>
+      </c>
+      <c r="O16">
+        <v>1.9724189999999999</v>
+      </c>
+      <c r="P16">
+        <v>134217728</v>
+      </c>
+      <c r="Q16">
+        <v>1.823731</v>
+      </c>
+      <c r="R16">
+        <v>134217728</v>
+      </c>
+      <c r="S16">
+        <v>1.756424</v>
+      </c>
+      <c r="T16">
+        <v>134217728</v>
+      </c>
+      <c r="U16">
+        <v>1.6717439999999999</v>
+      </c>
+      <c r="V16">
+        <v>134217728</v>
+      </c>
+      <c r="W16">
+        <v>1.6241019999999999</v>
+      </c>
+      <c r="X16">
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>27.775635000000001</v>
+      </c>
+      <c r="B17">
+        <v>268435456</v>
+      </c>
+      <c r="C17">
+        <v>14.656040000000001</v>
+      </c>
+      <c r="D17">
+        <v>268435456</v>
+      </c>
+      <c r="E17">
+        <v>9.9982500000000005</v>
+      </c>
+      <c r="F17">
+        <v>268435456</v>
+      </c>
+      <c r="G17">
+        <v>7.7049120000000002</v>
+      </c>
+      <c r="H17">
+        <v>268435456</v>
+      </c>
+      <c r="I17">
+        <v>6.392957</v>
+      </c>
+      <c r="J17">
+        <v>268435456</v>
+      </c>
+      <c r="K17">
+        <v>5.7343780000000004</v>
+      </c>
+      <c r="L17">
+        <v>268435456</v>
+      </c>
+      <c r="M17">
+        <v>5.0930150000000003</v>
+      </c>
+      <c r="N17">
+        <v>268435456</v>
+      </c>
+      <c r="O17">
+        <v>4.7942020000000003</v>
+      </c>
+      <c r="P17">
+        <v>268435456</v>
+      </c>
+      <c r="Q17">
+        <v>4.4864620000000004</v>
+      </c>
+      <c r="R17">
+        <v>268435456</v>
+      </c>
+      <c r="S17">
+        <v>4.2750810000000001</v>
+      </c>
+      <c r="T17">
+        <v>268435456</v>
+      </c>
+      <c r="U17">
+        <v>4.1199630000000003</v>
+      </c>
+      <c r="V17">
+        <v>268435456</v>
+      </c>
+      <c r="W17">
+        <v>3.9908800000000002</v>
+      </c>
+      <c r="X17">
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>80.702843000000001</v>
+      </c>
+      <c r="B18">
+        <v>536870912</v>
+      </c>
+      <c r="C18">
+        <v>41.039107000000001</v>
+      </c>
+      <c r="D18">
+        <v>536870912</v>
+      </c>
+      <c r="E18">
+        <v>29.173431999999998</v>
+      </c>
+      <c r="F18">
+        <v>536870912</v>
+      </c>
+      <c r="G18">
+        <v>22.372454999999999</v>
+      </c>
+      <c r="H18">
+        <v>536870912</v>
+      </c>
+      <c r="I18">
+        <v>18.725169000000001</v>
+      </c>
+      <c r="J18">
+        <v>536870912</v>
+      </c>
+      <c r="K18">
+        <v>16.374472999999998</v>
+      </c>
+      <c r="L18">
+        <v>536870912</v>
+      </c>
+      <c r="M18">
+        <v>14.725318</v>
+      </c>
+      <c r="N18">
+        <v>536870912</v>
+      </c>
+      <c r="O18">
+        <v>13.763139000000001</v>
+      </c>
+      <c r="P18">
+        <v>536870912</v>
+      </c>
+      <c r="Q18">
+        <v>12.877071000000001</v>
+      </c>
+      <c r="R18">
+        <v>536870912</v>
+      </c>
+      <c r="S18">
+        <v>12.158469</v>
+      </c>
+      <c r="T18">
+        <v>536870912</v>
+      </c>
+      <c r="U18">
+        <v>11.788122</v>
+      </c>
+      <c r="V18">
+        <v>536870912</v>
+      </c>
+      <c r="W18">
+        <v>11.341319</v>
+      </c>
+      <c r="X18">
+        <v>536870912</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K108"/>
   <sheetViews>
@@ -17604,7 +18958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C64351-AC61-47E3-95EB-BD879F3F42AB}">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -18539,12 +19893,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF50EC1-E23C-4024-AF4F-A049BCA5901E}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19392,7 +20746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD21AE94-B6F5-4D64-8047-7F7D73829D58}">
   <dimension ref="A1:B1002"/>
   <sheetViews>
@@ -27421,17 +28775,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35037BC3-A634-4EF6-BB0B-3D6FDEB96EA3}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -27559,7 +28914,7 @@
         <v>3276800</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.115623</v>
       </c>
@@ -27567,7 +28922,7 @@
         <v>6553600</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.123025</v>
       </c>
@@ -27575,7 +28930,7 @@
         <v>13107200</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.25098300000000001</v>
       </c>
@@ -27583,7 +28938,7 @@
         <v>26214400</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.550902</v>
       </c>
@@ -27591,7 +28946,7 @@
         <v>52428800</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.2648740000000001</v>
       </c>
@@ -27599,7 +28954,7 @@
         <v>104857600</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.9981499999999999</v>
       </c>
@@ -27607,7 +28962,7 @@
         <v>209715200</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7.6194610000000003</v>
       </c>
@@ -27615,7 +28970,7 @@
         <v>419430400</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>39.339447</v>
       </c>
@@ -27623,11 +28978,14 @@
         <v>838860800</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>360.39765399999999</v>
       </c>
       <c r="B25">
+        <v>1677721600</v>
+      </c>
+      <c r="C25" s="1">
         <v>1677721600</v>
       </c>
     </row>

</xml_diff>